<commit_message>
javedsheikh: hlookup and documentadd for v and h lookup
</commit_message>
<xml_diff>
--- a/Day_12.xlsx
+++ b/Day_12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F2C80E-5234-4596-85ED-795AEFCD8C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7277E197-CD0C-40BF-9A55-719BD5CDBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{343BB7B5-69E7-4B0B-AF2C-6DB97ACCEDA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{343BB7B5-69E7-4B0B-AF2C-6DB97ACCEDA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
   <si>
     <t>shop_name</t>
   </si>
@@ -587,7 +587,7 @@
         <v>1000</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" ref="H7:H12" si="0">VLOOKUP(C7,K$5:M$11,3,FALSE)</f>
+        <f t="shared" ref="H7:H11" si="0">VLOOKUP(C7,K$5:M$11,3,FALSE)</f>
         <v>10000</v>
       </c>
       <c r="I7" s="3">
@@ -754,10 +754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE74774D-67A2-4803-9FB1-99346A41E503}">
-  <dimension ref="C1:I15"/>
+  <dimension ref="C1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,22 +824,28 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
+      <c r="D5" s="1" t="str">
+        <f>HLOOKUP(D3,$C$17:$I$19,2,FALSE)</f>
+        <v>bhande plot</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" ref="E5:I5" si="1">HLOOKUP(E3,$C$17:$I$19,2,FALSE)</f>
+        <v>offline</v>
       </c>
       <c r="F5" s="1">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G5" s="1">
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="H5" s="1">
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="I5" s="1">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -871,11 +877,11 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f t="shared" ref="D7:E7" si="1">HLOOKUP(D3,$C$13:$I$15,3,FALSE)</f>
+        <f t="shared" ref="D7:E7" si="2">HLOOKUP(D3,$C$13:$I$15,3,FALSE)</f>
         <v>nandanvan</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>online</v>
       </c>
       <c r="F7" s="1">
@@ -883,15 +889,15 @@
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:I7" si="2">HLOOKUP(G3,$C$13:$I$15,3,FALSE)</f>
+        <f t="shared" ref="G7:I7" si="3">HLOOKUP(G3,$C$13:$I$15,3,FALSE)</f>
         <v>15000</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200000</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
     </row>
@@ -899,22 +905,28 @@
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
+      <c r="D8" s="1" t="str">
+        <f t="shared" ref="D8:E8" si="4">HLOOKUP(D3,$C$17:$I$19,3,FALSE)</f>
+        <v xml:space="preserve">wardhman </v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>online</v>
       </c>
       <c r="F8" s="1">
+        <f>HLOOKUP(F3,$C$17:$I$19,3,FALSE)</f>
         <v>3</v>
       </c>
       <c r="G8" s="1">
+        <f t="shared" ref="G8:I8" si="5">HLOOKUP(G3,$C$17:$I$19,3,FALSE)</f>
         <v>12000</v>
       </c>
       <c r="H8" s="1">
+        <f t="shared" si="5"/>
         <v>150000</v>
       </c>
       <c r="I8" s="1">
+        <f t="shared" si="5"/>
         <v>7000</v>
       </c>
     </row>
@@ -1008,6 +1020,75 @@
       </c>
       <c r="I15" s="1">
         <v>15000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>100</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7000</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>150000</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
javedsheikh: vlookup and hlookup task complete
</commit_message>
<xml_diff>
--- a/Day_12.xlsx
+++ b/Day_12.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7277E197-CD0C-40BF-9A55-719BD5CDBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA0E1C-6CD4-49D9-95A6-9A9FB0D0DDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{343BB7B5-69E7-4B0B-AF2C-6DB97ACCEDA2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Vlookup" sheetId="1" r:id="rId1"/>
+    <sheet name="Hlookup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
   <si>
     <t>shop_name</t>
   </si>
@@ -101,6 +101,63 @@
   </si>
   <si>
     <t>vlookup</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A.1</t>
+  </si>
+  <si>
+    <t>A.2</t>
+  </si>
+  <si>
+    <t>A.3</t>
+  </si>
+  <si>
+    <t>A.4</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>E.1</t>
+  </si>
+  <si>
+    <t>E.2</t>
+  </si>
+  <si>
+    <t>E.3</t>
+  </si>
+  <si>
+    <t>E.4</t>
   </si>
 </sst>
 </file>
@@ -485,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DFD416-6ABE-49E8-B3FB-657236B18037}">
-  <dimension ref="C5:M12"/>
+  <dimension ref="A5:P26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +560,7 @@
     <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
@@ -569,7 +626,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
@@ -603,7 +660,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
@@ -637,7 +694,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
@@ -671,7 +728,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
@@ -705,7 +762,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
@@ -739,12 +796,366 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>21</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1">
+        <f>VLOOKUP(C16,$N$15:$P$19,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="G16" s="1">
+        <f>VLOOKUP(C16,$N$15:$P$19,3,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="H16" s="1">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1">
+        <v>50</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="1">
+        <v>10</v>
+      </c>
+      <c r="P16" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:F19" si="2">VLOOKUP(C17,N$15:P$19,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17:G20" si="3">VLOOKUP(C17,$N$15:$P$19,3,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="1">
+        <v>7</v>
+      </c>
+      <c r="P17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>9</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="1">
+        <v>7</v>
+      </c>
+      <c r="P18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H19" s="1">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1">
+        <v>25</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="1">
+        <v>14</v>
+      </c>
+      <c r="P19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1">
+        <v>50</v>
+      </c>
+      <c r="E23" s="1">
+        <f>VLOOKUP(C23,N$22:P$26,2,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="F23" s="1">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1">
+        <v>47</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H25" si="4">VLOOKUP(C23,N$22:P$26,3,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="I23" s="1">
+        <v>40</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" s="1">
+        <v>40</v>
+      </c>
+      <c r="P23" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1">
+        <v>47</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" ref="E24:E26" si="5">VLOOKUP(C24,N$22:P$26,2,FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="F24" s="1">
+        <v>67</v>
+      </c>
+      <c r="G24" s="1">
+        <v>69</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="I24" s="1">
+        <v>80</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="1">
+        <v>60</v>
+      </c>
+      <c r="P24" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1">
+        <v>80</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="F25" s="1">
+        <v>90</v>
+      </c>
+      <c r="G25" s="1">
+        <v>97</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="I25" s="1">
+        <v>88</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O25" s="1">
+        <v>41</v>
+      </c>
+      <c r="P25" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="F26" s="1">
+        <v>23</v>
+      </c>
+      <c r="G26" s="1">
+        <v>46</v>
+      </c>
+      <c r="H26" s="1">
+        <f>VLOOKUP(C26,N$22:P$26,3,FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="I26" s="1">
+        <v>25</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O26" s="1">
+        <v>21</v>
+      </c>
+      <c r="P26" s="1">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -754,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE74774D-67A2-4803-9FB1-99346A41E503}">
-  <dimension ref="C1:I19"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,8 +1178,8 @@
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -791,7 +1202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -820,7 +1231,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
@@ -849,7 +1260,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
@@ -872,7 +1283,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
@@ -901,7 +1312,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
@@ -930,7 +1341,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
@@ -953,7 +1364,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
@@ -976,7 +1392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1415,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1022,7 +1438,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1484,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1089,6 +1505,396 @@
       </c>
       <c r="I19" s="1">
         <v>12000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="1">
+        <f>HLOOKUP(D22,$L$23:$R$24,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" ref="E23:I23" si="6">HLOOKUP(E22,$L$23:$R$24,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="1">
+        <v>30</v>
+      </c>
+      <c r="N24" s="1">
+        <v>50</v>
+      </c>
+      <c r="O24" s="1">
+        <v>15</v>
+      </c>
+      <c r="P24" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>40</v>
+      </c>
+      <c r="R24" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4</v>
+      </c>
+      <c r="I25" s="1">
+        <v>9</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="1">
+        <v>15</v>
+      </c>
+      <c r="N25" s="1">
+        <v>25</v>
+      </c>
+      <c r="O25" s="1">
+        <v>10</v>
+      </c>
+      <c r="P25" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>20</v>
+      </c>
+      <c r="R25" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" ref="D26:E26" si="7">HLOOKUP(D22,$L$23:$R$25,3,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="F26" s="1">
+        <f>HLOOKUP(F22,$L$23:$R$25,3,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" ref="G26:I26" si="8">HLOOKUP(G22,$L$23:$R$25,3,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="1">
+        <f>HLOOKUP(D29,$L$29:$R$31,2,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" ref="E30:I30" si="9">HLOOKUP(E29,$L$29:$R$31,2,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="9"/>
+        <v>47</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30" s="1">
+        <v>55</v>
+      </c>
+      <c r="N30" s="1">
+        <v>39</v>
+      </c>
+      <c r="O30" s="1">
+        <v>40</v>
+      </c>
+      <c r="P30" s="1">
+        <v>47</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>50</v>
+      </c>
+      <c r="R30" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1">
+        <v>47</v>
+      </c>
+      <c r="E31" s="1">
+        <v>60</v>
+      </c>
+      <c r="F31" s="1">
+        <v>67</v>
+      </c>
+      <c r="G31" s="1">
+        <v>69</v>
+      </c>
+      <c r="H31" s="1">
+        <v>75</v>
+      </c>
+      <c r="I31" s="1">
+        <v>80</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="1">
+        <v>90</v>
+      </c>
+      <c r="N31" s="1">
+        <v>98</v>
+      </c>
+      <c r="O31" s="1">
+        <v>88</v>
+      </c>
+      <c r="P31" s="1">
+        <v>97</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>80</v>
+      </c>
+      <c r="R31" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" ref="D32:H32" si="10">HLOOKUP(D29,$L$29:$R$31,3,FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="10"/>
+        <v>41</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="10"/>
+        <v>97</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="10"/>
+        <v>98</v>
+      </c>
+      <c r="I32" s="1">
+        <f>HLOOKUP(I29,$L$29:$R$31,3,FALSE)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1">
+        <v>21</v>
+      </c>
+      <c r="F33" s="1">
+        <v>23</v>
+      </c>
+      <c r="G33" s="1">
+        <v>46</v>
+      </c>
+      <c r="H33" s="1">
+        <v>47</v>
+      </c>
+      <c r="I33" s="1">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>